<commit_message>
accuracy of id is perfect now
</commit_message>
<xml_diff>
--- a/Student_Results.xlsx
+++ b/Student_Results.xlsx
@@ -977,7 +977,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5#</t>
+          <t>54</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1023,7 +1023,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>7#</t>
+          <t>78</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1069,7 +1069,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>8#</t>
+          <t>89</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1115,7 +1115,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>##</t>
+          <t>01</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1161,7 +1161,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4#</t>
+          <t>43</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1207,7 +1207,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>6#</t>
+          <t>69</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1253,7 +1253,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>##</t>
+          <t>06</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1299,7 +1299,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>##</t>
+          <t>90</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1345,7 +1345,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>##</t>
+          <t>9#</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1391,7 +1391,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>##</t>
+          <t>56</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1437,7 +1437,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>##</t>
+          <t>67</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1529,7 +1529,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>##</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1575,7 +1575,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>##</t>
+          <t>#3</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1621,7 +1621,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>199887#</t>
+          <t>1998876</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1763,7 +1763,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>####</t>
+          <t>0101</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1818,7 +1818,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>#####4#</t>
+          <t>1170044</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1879,7 +1879,7 @@
         <v>1</v>
       </c>
       <c r="U19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19" t="n">
         <v>1</v>
@@ -1888,7 +1888,7 @@
         <v>1</v>
       </c>
       <c r="X19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y19" t="n">
         <v>1</v>
@@ -1921,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="AI19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ19" t="n">
         <v>0</v>
@@ -1960,7 +1960,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>####</t>
+          <t>9998</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -2015,7 +2015,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4521</t>
+          <t>0521</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -2269,7 +2269,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>#343435</t>
+          <t>0099095</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -2411,7 +2411,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4#43435</t>
+          <t>8899908</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -2553,7 +2553,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>9999996</t>
+          <t>0099906</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -2695,7 +2695,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>9999996</t>
+          <t>9098096</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -2837,7 +2837,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>0###4##</t>
+          <t>0983456</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -2979,7 +2979,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>11#1111</t>
+          <t>9099011</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -3121,7 +3121,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1##1#11</t>
+          <t>0000111</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -3263,7 +3263,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6666669</t>
+          <t>0666669</t>
         </is>
       </c>
       <c r="B30" t="n">

</xml_diff>

<commit_message>
The best accuracy for all the files (id and questions)
</commit_message>
<xml_diff>
--- a/Student_Results.xlsx
+++ b/Student_Results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CW30"/>
+  <dimension ref="A1:CW39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1888,7 +1888,7 @@
         <v>1</v>
       </c>
       <c r="X19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y19" t="n">
         <v>1</v>
@@ -1921,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="AI19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ19" t="n">
         <v>0</v>
@@ -3263,7 +3263,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>0666669</t>
+          <t>0966669</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -3399,6 +3399,762 @@
         <v>1</v>
       </c>
       <c r="AT30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>6333333</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="n">
+        <v>1</v>
+      </c>
+      <c r="S31" t="n">
+        <v>1</v>
+      </c>
+      <c r="T31" t="n">
+        <v>1</v>
+      </c>
+      <c r="U31" t="n">
+        <v>1</v>
+      </c>
+      <c r="V31" t="n">
+        <v>1</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>9600220</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>1</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>1</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="n">
+        <v>1</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>0090000</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>1</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>1</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>1</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>1</v>
+      </c>
+      <c r="U33" t="n">
+        <v>1</v>
+      </c>
+      <c r="V33" t="n">
+        <v>1</v>
+      </c>
+      <c r="W33" t="n">
+        <v>1</v>
+      </c>
+      <c r="X33" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2189</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" t="n">
+        <v>1</v>
+      </c>
+      <c r="K34" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" t="n">
+        <v>1</v>
+      </c>
+      <c r="M34" t="n">
+        <v>1</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>5555</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" t="n">
+        <v>1</v>
+      </c>
+      <c r="K35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M35" t="n">
+        <v>1</v>
+      </c>
+      <c r="N35" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" t="n">
+        <v>1</v>
+      </c>
+      <c r="P35" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2222</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J36" t="n">
+        <v>1</v>
+      </c>
+      <c r="K36" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" t="n">
+        <v>1</v>
+      </c>
+      <c r="M36" t="n">
+        <v>1</v>
+      </c>
+      <c r="N36" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" t="n">
+        <v>1</v>
+      </c>
+      <c r="P36" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>088#</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>1</v>
+      </c>
+      <c r="O37" t="n">
+        <v>1</v>
+      </c>
+      <c r="P37" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>0991</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>0234</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>1</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1</v>
+      </c>
+      <c r="K39" t="n">
+        <v>1</v>
+      </c>
+      <c r="L39" t="n">
+        <v>1</v>
+      </c>
+      <c r="M39" t="n">
+        <v>1</v>
+      </c>
+      <c r="N39" t="n">
+        <v>1</v>
+      </c>
+      <c r="O39" t="n">
+        <v>1</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>